<commit_message>
UpdatePCB and some code
</commit_message>
<xml_diff>
--- a/Docs/Work.xlsx
+++ b/Docs/Work.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\Khoaluan\Khoaluan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\Khoaluan\Khoaluan\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43E8038-27C7-458F-A251-8E0EDF95B53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAA5A98-A035-4540-9A7D-9A316FE57FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{10090A17-CE37-4630-85BF-5843CA0553E4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="72">
   <si>
     <t>STT</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>v</t>
+  </si>
+  <si>
+    <t>Lưu thời gian</t>
+  </si>
+  <si>
+    <t>Không được xóa địa chỉ này về 0</t>
   </si>
 </sst>
 </file>
@@ -308,10 +314,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1148,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7602F501-B38D-4F09-983B-106FCB899D33}">
-  <dimension ref="A2:K12"/>
+  <dimension ref="A2:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1167,7 +1174,7 @@
     <col min="11" max="11" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1206,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1233,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1270,7 +1277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1304,7 +1311,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1338,7 +1345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1371,11 +1378,11 @@
         <v>6</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" ref="K7:K12" si="2">(G7+J7)-1</f>
+        <f t="shared" ref="K7:K13" si="2">(G7+J7)-1</f>
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1412,7 +1419,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1441,7 +1448,7 @@
         <v>4</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" ref="J9:J12" si="3">H9*I9</f>
+        <f t="shared" ref="J9:J13" si="3">H9*I9</f>
         <v>80</v>
       </c>
       <c r="K9" s="1">
@@ -1449,7 +1456,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1486,7 +1493,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>51</v>
       </c>
@@ -1514,7 +1521,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F12" s="1" t="s">
         <v>59</v>
       </c>
@@ -1534,6 +1541,31 @@
       <c r="K12" s="1">
         <f t="shared" si="2"/>
         <v>499</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="3">
+        <v>520</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K13" s="3">
+        <f>(G13+J13)-1</f>
+        <v>520</v>
+      </c>
+      <c r="L13" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>